<commit_message>
corrected numbers of upset figures
</commit_message>
<xml_diff>
--- a/tables/mfp.upset.matrix.xlsx
+++ b/tables/mfp.upset.matrix.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">miRNA</t>
   </si>
@@ -93,6 +93,51 @@
   </si>
   <si>
     <t xml:space="preserve">mmu-miR-449c-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-143-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-133a-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-129-2-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-129-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-434-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-10b-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-27a-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-7036-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-7a-2-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-1a-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-133b-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-668-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-541-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-184-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmu-miR-6414</t>
   </si>
 </sst>
 </file>
@@ -907,6 +952,351 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>